<commit_message>
atc model added with an example
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>TP</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>DE</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>Zone (from)</t>
@@ -431,10 +434,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="C2">
-        <v>-350</v>
+        <v>-400</v>
       </c>
     </row>
   </sheetData>
@@ -480,8 +483,8 @@
       <c r="D2">
         <v>-50</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -495,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-100</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+        <v>-150</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -509,13 +512,13 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D4">
         <v>-200</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -533,16 +536,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -556,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -570,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>